<commit_message>
Final version of code, Question to answer with the analysis
</commit_message>
<xml_diff>
--- a/Datasets/Treated/GDP-Growth_Europe.xlsx
+++ b/Datasets/Treated/GDP-Growth_Europe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppcro\Desktop\Universidade\Mestrado\1º ano\2º Semestre\Sistemas de Gestão de Dados\PA-Statistical Analysis\SGD_Data-Analysis\Datasets\Treated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DB75BD-BBB3-45A0-9221-92A7E6320FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28003BB2-2B56-490C-9753-7DA9CEDD1D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3828" yWindow="2940" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Serbia</t>
   </si>
   <si>
-    <t>Türkiye</t>
-  </si>
-  <si>
     <t>Ukraine</t>
   </si>
   <si>
@@ -151,14 +148,25 @@
   </si>
   <si>
     <t>Country Name</t>
+  </si>
+  <si>
+    <t>Turkey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -186,8 +194,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,17 +477,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1">
         <v>2013</v>
@@ -1788,7 +1797,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1829,7 +1838,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1869,8 +1878,9 @@
       <c r="M34">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q34" s="1"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1911,7 +1921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1952,7 +1962,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1993,7 +2003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2034,9 +2044,9 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>8.5</v>
@@ -2075,9 +2085,9 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2116,9 +2126,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>5.3</v>

</xml_diff>